<commit_message>
MAJ + nouveau script 30_application_criteres_lrr + remise à jour des excel concernant les temps de générations et caractère endémique des différents poissons.
</commit_message>
<xml_diff>
--- a/raw_data/traits_biologiques.xlsx
+++ b/raw_data/traits_biologiques.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20408"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lea.bouchet\Documents\Artif\Artif\liste_rouge_regionale\raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F814421D-44F3-4729-A619-840F03D1A4AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2BA2389-7930-41A5-BEE4-414E7B4227D5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{25E8E10F-A282-45EE-82C4-3240378E5878}"/>
   </bookViews>
@@ -354,9 +354,6 @@
     <t>taille_min</t>
   </si>
   <si>
-    <t>duree_generation</t>
-  </si>
-  <si>
     <t>VAR</t>
   </si>
   <si>
@@ -394,6 +391,9 @@
   </si>
   <si>
     <t>Chevesne</t>
+  </si>
+  <si>
+    <t>temps_generation</t>
   </si>
 </sst>
 </file>
@@ -805,13 +805,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68C65F63-35D5-4CD1-B443-72BB0835CA8F}">
   <dimension ref="A1:L598"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B34" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="J41" sqref="J41"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="26.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="17.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" style="1" customWidth="1"/>
@@ -827,7 +827,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>102</v>
@@ -851,13 +851,13 @@
         <v>101</v>
       </c>
       <c r="I1" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="J1" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="J1" s="11" t="s">
-        <v>112</v>
-      </c>
       <c r="K1" s="5" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="L1" s="6" t="s">
         <v>107</v>
@@ -941,9 +941,6 @@
         <v>50</v>
       </c>
       <c r="J4" s="1"/>
-      <c r="K4" s="1">
-        <v>3</v>
-      </c>
       <c r="L4" s="1">
         <v>400</v>
       </c>
@@ -974,9 +971,6 @@
         <v>170</v>
       </c>
       <c r="J5" s="1"/>
-      <c r="K5" s="1">
-        <v>15</v>
-      </c>
       <c r="L5" s="1">
         <v>250</v>
       </c>
@@ -1009,9 +1003,6 @@
         <v>40.5</v>
       </c>
       <c r="J6" s="1"/>
-      <c r="K6" s="1">
-        <v>3</v>
-      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -1066,9 +1057,6 @@
         <v>225</v>
       </c>
       <c r="J8" s="1"/>
-      <c r="K8" s="1">
-        <v>10</v>
-      </c>
       <c r="L8" s="1">
         <v>50</v>
       </c>
@@ -1211,16 +1199,13 @@
         <v>38</v>
       </c>
       <c r="J13" s="1"/>
-      <c r="K13" s="1">
-        <v>3</v>
-      </c>
       <c r="L13" s="1">
         <v>500</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>22</v>
@@ -1242,10 +1227,7 @@
         <v>57.5</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="K14" s="1">
-        <v>5</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1274,9 +1256,6 @@
         <v>300</v>
       </c>
       <c r="J15" s="1"/>
-      <c r="K15" s="1">
-        <v>15</v>
-      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
@@ -1306,9 +1285,6 @@
         <v>200</v>
       </c>
       <c r="J16" s="1"/>
-      <c r="K16" s="1">
-        <v>6</v>
-      </c>
       <c r="L16" s="1">
         <v>250</v>
       </c>
@@ -1341,9 +1317,6 @@
         <v>80</v>
       </c>
       <c r="J17" s="1"/>
-      <c r="K17" s="1">
-        <v>5</v>
-      </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
@@ -1427,9 +1400,6 @@
         <v>300</v>
       </c>
       <c r="J20" s="1"/>
-      <c r="K20" s="1">
-        <v>15</v>
-      </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
@@ -1484,9 +1454,6 @@
         <v>700</v>
       </c>
       <c r="J22" s="1"/>
-      <c r="K22" s="1">
-        <v>20</v>
-      </c>
       <c r="L22" s="1">
         <v>25</v>
       </c>
@@ -1519,9 +1486,6 @@
         <v>100</v>
       </c>
       <c r="J23" s="1"/>
-      <c r="K23" s="1">
-        <v>3</v>
-      </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
@@ -1584,9 +1548,6 @@
         <v>290</v>
       </c>
       <c r="J25" s="1"/>
-      <c r="K25" s="1">
-        <v>3</v>
-      </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
@@ -1618,10 +1579,10 @@
         <v>100</v>
       </c>
       <c r="J26" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K26" s="1">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="L26" s="1">
         <v>110</v>
@@ -1653,7 +1614,7 @@
       </c>
       <c r="J27" s="1"/>
       <c r="K27" s="1">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="L27" s="1">
         <v>25</v>
@@ -1683,9 +1644,6 @@
         <v>465</v>
       </c>
       <c r="J28" s="1"/>
-      <c r="K28" s="1">
-        <v>5</v>
-      </c>
       <c r="L28" s="1">
         <v>50</v>
       </c>
@@ -1718,7 +1676,7 @@
       </c>
       <c r="J29" s="1"/>
       <c r="K29" s="1">
-        <v>12</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -1751,10 +1709,10 @@
         <v>200</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K30" s="1">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -1786,10 +1744,10 @@
         <v>280</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K31" s="1">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="L31" s="1">
         <v>50</v>
@@ -1825,7 +1783,7 @@
       </c>
       <c r="J32" s="1"/>
       <c r="K32" s="1">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="L32" s="1">
         <v>700</v>
@@ -1861,10 +1819,10 @@
         <v>450</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K33" s="1">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="L33" s="1">
         <v>90</v>
@@ -1900,10 +1858,10 @@
         <v>50</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K34" s="1">
-        <v>3.5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
@@ -1911,7 +1869,7 @@
         <v>1</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>77</v>
@@ -1935,10 +1893,10 @@
         <v>300</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K35" s="1">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="L35" s="1">
         <v>300</v>
@@ -1972,10 +1930,10 @@
         <v>34</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K36" s="1">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
@@ -2004,10 +1962,10 @@
         <v>40</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K37" s="1">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="L37" s="1">
         <v>150</v>
@@ -2041,9 +1999,6 @@
         <v>215</v>
       </c>
       <c r="J38" s="1"/>
-      <c r="K38" s="1">
-        <v>3</v>
-      </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
@@ -2075,10 +2030,10 @@
         <v>57</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K39" s="1">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
@@ -2111,10 +2066,10 @@
         <v>100</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K40" s="1">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
@@ -2145,10 +2100,10 @@
         <v>65</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K41" s="1">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="L41" s="1">
         <v>50</v>
@@ -2179,9 +2134,6 @@
         <v>750</v>
       </c>
       <c r="J42" s="1"/>
-      <c r="K42" s="1">
-        <v>3</v>
-      </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
@@ -2213,10 +2165,10 @@
         <v>150</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K43" s="1">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="L43" s="1">
         <v>450</v>
@@ -2279,9 +2231,6 @@
         <v>270</v>
       </c>
       <c r="J45" s="1"/>
-      <c r="K45" s="1">
-        <v>3</v>
-      </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
@@ -2314,7 +2263,7 @@
       </c>
       <c r="J46" s="1"/>
       <c r="K46" s="1">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="L46" s="1">
         <v>50</v>
@@ -2347,10 +2296,10 @@
         <v>100</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K47" s="1">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
@@ -2379,7 +2328,7 @@
       </c>
       <c r="J48" s="1"/>
       <c r="K48" s="1">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
@@ -2410,10 +2359,10 @@
         <v>240</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K49" s="1">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
@@ -2445,10 +2394,10 @@
         <v>200</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K50" s="1">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
@@ -2479,10 +2428,10 @@
         <v>70</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K51" s="1">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
@@ -2493,7 +2442,7 @@
         <v>44</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D52" s="8">
         <v>110</v>
@@ -2514,10 +2463,10 @@
         <v>170</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K52" s="1">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="L52" s="1">
         <v>150</v>

</xml_diff>

<commit_message>
MAJ - 05-06 soir
</commit_message>
<xml_diff>
--- a/raw_data/traits_biologiques.xlsx
+++ b/raw_data/traits_biologiques.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lea.bouchet\Documents\Artif\Artif\liste_rouge_regionale\raw_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lea.bouchet\Documents\Artif\Artif\liste_rouge_regionale_old\raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2BA2389-7930-41A5-BEE4-414E7B4227D5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4528C03F-BE1E-4C70-9429-57C67638A2DA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{25E8E10F-A282-45EE-82C4-3240378E5878}"/>
   </bookViews>
@@ -360,9 +360,6 @@
     <t>espece_presence_lrr_2015</t>
   </si>
   <si>
-    <t>taille_maturite</t>
-  </si>
-  <si>
     <t>age_maturite</t>
   </si>
   <si>
@@ -394,6 +391,9 @@
   </si>
   <si>
     <t>temps_generation</t>
+  </si>
+  <si>
+    <t>taille_maturite_ref</t>
   </si>
 </sst>
 </file>
@@ -805,8 +805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68C65F63-35D5-4CD1-B443-72BB0835CA8F}">
   <dimension ref="A1:L598"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -851,13 +851,13 @@
         <v>101</v>
       </c>
       <c r="I1" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="J1" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="J1" s="11" t="s">
-        <v>111</v>
-      </c>
       <c r="K1" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L1" s="6" t="s">
         <v>107</v>
@@ -1227,7 +1227,7 @@
         <v>57.5</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1579,7 +1579,7 @@
         <v>100</v>
       </c>
       <c r="J26" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K26" s="1">
         <v>15</v>
@@ -1709,7 +1709,7 @@
         <v>200</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K30" s="1">
         <v>12</v>
@@ -1744,7 +1744,7 @@
         <v>280</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K31" s="1">
         <v>15</v>
@@ -1819,7 +1819,7 @@
         <v>450</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K33" s="1">
         <v>15</v>
@@ -1858,7 +1858,7 @@
         <v>50</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K34" s="1">
         <v>10</v>
@@ -1869,7 +1869,7 @@
         <v>1</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>77</v>
@@ -1893,7 +1893,7 @@
         <v>300</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K35" s="1">
         <v>18</v>
@@ -1930,7 +1930,7 @@
         <v>34</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K36" s="1">
         <v>10</v>
@@ -1962,7 +1962,7 @@
         <v>40</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K37" s="1">
         <v>10</v>
@@ -2030,7 +2030,7 @@
         <v>57</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K39" s="1">
         <v>12</v>
@@ -2066,7 +2066,7 @@
         <v>100</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K40" s="1">
         <v>10</v>
@@ -2100,7 +2100,7 @@
         <v>65</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K41" s="1">
         <v>15</v>
@@ -2165,7 +2165,7 @@
         <v>150</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K43" s="1">
         <v>18</v>
@@ -2296,7 +2296,7 @@
         <v>100</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K47" s="1">
         <v>15</v>
@@ -2359,7 +2359,7 @@
         <v>240</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K49" s="1">
         <v>15</v>
@@ -2394,7 +2394,7 @@
         <v>200</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K50" s="1">
         <v>10</v>
@@ -2428,7 +2428,7 @@
         <v>70</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K51" s="1">
         <v>12</v>
@@ -2463,7 +2463,7 @@
         <v>170</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K52" s="1">
         <v>12</v>

</xml_diff>